<commit_message>
The first row of the excel file is getting updated
</commit_message>
<xml_diff>
--- a/Weather/newFile.xlsx
+++ b/Weather/newFile.xlsx
@@ -12,9 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>string</t>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>Wind Speed</t>
   </si>
 </sst>
 </file>
@@ -59,27 +68,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1.4</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="n">
-        <v>7.0</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" t="n">
-        <v>99.0</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
-      <c r="E1" t="b">
-        <v>1</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>301.20001220703125</v>
+      </c>
+      <c r="B2" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1012.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.099999904632568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>